<commit_message>
Add installation instructions. Make filepaths platform-independent
</commit_message>
<xml_diff>
--- a/modules/G/Document weights.xlsx
+++ b/modules/G/Document weights.xlsx
@@ -534,16 +534,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>31.75272172447578</v>
+        <v>127.0108868979071</v>
       </c>
       <c r="C2">
-        <v>1534</v>
+        <v>6136</v>
       </c>
       <c r="D2">
-        <v>0.02069929708244836</v>
+        <v>0.020699297082449</v>
       </c>
       <c r="E2">
-        <v>31.75272172447578</v>
+        <v>127.0108868979071</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -551,16 +551,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>-15.31153004641834</v>
+        <v>-61.24612018567306</v>
       </c>
       <c r="C3">
-        <v>183</v>
+        <v>732</v>
       </c>
       <c r="D3">
-        <v>-0.08366956309518217</v>
+        <v>-0.08366956309518178</v>
       </c>
       <c r="E3">
-        <v>-15.31153004641834</v>
+        <v>-61.24612018567306</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -568,16 +568,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>-53.08546190525055</v>
+        <v>-212.3418476210031</v>
       </c>
       <c r="C4">
-        <v>976</v>
+        <v>3904</v>
       </c>
       <c r="D4">
-        <v>-0.0543908421160354</v>
+        <v>-0.05439084211603563</v>
       </c>
       <c r="E4">
-        <v>-53.08546190525055</v>
+        <v>-212.3418476210031</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -585,16 +585,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>-20.81476007907387</v>
+        <v>-83.25904031629506</v>
       </c>
       <c r="C5">
-        <v>361</v>
+        <v>1444</v>
       </c>
       <c r="D5">
-        <v>-0.05765861517748994</v>
+        <v>-0.05765861517748965</v>
       </c>
       <c r="E5">
-        <v>-20.81476007907387</v>
+        <v>-83.25904031629506</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -602,16 +602,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>-95.4617377533832</v>
+        <v>-381.8469510135291</v>
       </c>
       <c r="C6">
-        <v>936</v>
+        <v>3744</v>
       </c>
       <c r="D6">
-        <v>-0.1019890360613068</v>
+        <v>-0.1019890360613059</v>
       </c>
       <c r="E6">
-        <v>-95.4617377533832</v>
+        <v>-381.8469510135291</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -619,16 +619,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>-56.74379483827924</v>
+        <v>-226.9751793531174</v>
       </c>
       <c r="C7">
-        <v>848</v>
+        <v>3392</v>
       </c>
       <c r="D7">
-        <v>-0.06691485240363118</v>
+        <v>-0.06691485240363132</v>
       </c>
       <c r="E7">
-        <v>-56.74379483827924</v>
+        <v>-226.9751793531174</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -636,16 +636,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>-39.22190392371704</v>
+        <v>-156.8876156948677</v>
       </c>
       <c r="C8">
-        <v>824</v>
+        <v>3296</v>
       </c>
       <c r="D8">
-        <v>-0.04759939796567601</v>
+        <v>-0.0475993979656759</v>
       </c>
       <c r="E8">
-        <v>-39.22190392371704</v>
+        <v>-156.8876156948677</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -653,16 +653,16 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>-20.58234184288479</v>
+        <v>-82.32936737153875</v>
       </c>
       <c r="C9">
-        <v>981</v>
+        <v>3924</v>
       </c>
       <c r="D9">
-        <v>-0.02098098047184994</v>
+        <v>-0.02098098047184983</v>
       </c>
       <c r="E9">
-        <v>-20.58234184288479</v>
+        <v>-82.32936737153875</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -670,16 +670,16 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>9.295487768645371</v>
+        <v>37.18195107458128</v>
       </c>
       <c r="C10">
-        <v>408</v>
+        <v>1632</v>
       </c>
       <c r="D10">
-        <v>0.02278305825648375</v>
+        <v>0.02278305825648362</v>
       </c>
       <c r="E10">
-        <v>9.295487768645371</v>
+        <v>37.18195107458128</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -687,16 +687,16 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>-37.41568577156428</v>
+        <v>-149.662743086256</v>
       </c>
       <c r="C11">
-        <v>652</v>
+        <v>2608</v>
       </c>
       <c r="D11">
-        <v>-0.05738602112203111</v>
+        <v>-0.05738602112203069</v>
       </c>
       <c r="E11">
-        <v>-37.41568577156428</v>
+        <v>-149.662743086256</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -704,16 +704,16 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>-65.06157438938023</v>
+        <v>-260.2462975575222</v>
       </c>
       <c r="C12">
-        <v>461</v>
+        <v>1844</v>
       </c>
       <c r="D12">
-        <v>-0.1411313978077662</v>
+        <v>-0.1411313978077669</v>
       </c>
       <c r="E12">
-        <v>-65.06157438938023</v>
+        <v>-260.2462975575222</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -721,16 +721,16 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>-31.371975342209</v>
+        <v>-125.4879013688354</v>
       </c>
       <c r="C13">
-        <v>222</v>
+        <v>888</v>
       </c>
       <c r="D13">
-        <v>-0.1413152042441847</v>
+        <v>-0.141315204244184</v>
       </c>
       <c r="E13">
-        <v>-31.371975342209</v>
+        <v>-125.4879013688354</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -738,16 +738,16 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>11.37234831784946</v>
+        <v>45.489393271398</v>
       </c>
       <c r="C14">
-        <v>366</v>
+        <v>1464</v>
       </c>
       <c r="D14">
-        <v>0.03107198993947941</v>
+        <v>0.03107198993947951</v>
       </c>
       <c r="E14">
-        <v>11.37234831784946</v>
+        <v>45.489393271398</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -755,16 +755,16 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>-180.0147606267437</v>
+        <v>-720.0590425069661</v>
       </c>
       <c r="C15">
-        <v>1837</v>
+        <v>7348</v>
       </c>
       <c r="D15">
-        <v>-0.09799388166943042</v>
+        <v>-0.09799388166942924</v>
       </c>
       <c r="E15">
-        <v>-180.0147606267437</v>
+        <v>-720.0590425069661</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -772,16 +772,16 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>11.92723838502822</v>
+        <v>47.70895354011265</v>
       </c>
       <c r="C16">
-        <v>640</v>
+        <v>2560</v>
       </c>
       <c r="D16">
-        <v>0.0186363099766066</v>
+        <v>0.0186363099766065</v>
       </c>
       <c r="E16">
-        <v>11.92723838502822</v>
+        <v>47.70895354011265</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -789,16 +789,16 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>-148.7439466281327</v>
+        <v>-594.9757865125223</v>
       </c>
       <c r="C17">
-        <v>974</v>
+        <v>3896</v>
       </c>
       <c r="D17">
-        <v>-0.1527145242588632</v>
+        <v>-0.152714524258861</v>
       </c>
       <c r="E17">
-        <v>-148.7439466281327</v>
+        <v>-594.9757865125223</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -806,16 +806,16 @@
         <v>21</v>
       </c>
       <c r="B18">
-        <v>-8.234868724745295</v>
+        <v>-32.93947489898112</v>
       </c>
       <c r="C18">
-        <v>244</v>
+        <v>976</v>
       </c>
       <c r="D18">
-        <v>-0.03374946198666105</v>
+        <v>-0.03374946198666098</v>
       </c>
       <c r="E18">
-        <v>-8.234868724745295</v>
+        <v>-32.93947489898112</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -823,16 +823,16 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <v>-112.7175853406481</v>
+        <v>-450.8703413625891</v>
       </c>
       <c r="C19">
-        <v>1159</v>
+        <v>4636</v>
       </c>
       <c r="D19">
-        <v>-0.09725417199365671</v>
+        <v>-0.09725417199365598</v>
       </c>
       <c r="E19">
-        <v>-112.7175853406481</v>
+        <v>-450.8703413625891</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -840,16 +840,16 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>-28.17825250185301</v>
+        <v>-112.7130100074113</v>
       </c>
       <c r="C20">
-        <v>297</v>
+        <v>1188</v>
       </c>
       <c r="D20">
-        <v>-0.09487627105001015</v>
+        <v>-0.09487627105000955</v>
       </c>
       <c r="E20">
-        <v>-28.17825250185301</v>
+        <v>-112.7130100074113</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -857,16 +857,16 @@
         <v>24</v>
       </c>
       <c r="B21">
-        <v>-12.56574680623434</v>
+        <v>-50.26298722493762</v>
       </c>
       <c r="C21">
-        <v>563</v>
+        <v>2252</v>
       </c>
       <c r="D21">
-        <v>-0.02231926608567378</v>
+        <v>-0.0223192660856739</v>
       </c>
       <c r="E21">
-        <v>-12.56574680623434</v>
+        <v>-50.26298722493762</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -874,16 +874,16 @@
         <v>25</v>
       </c>
       <c r="B22">
-        <v>-27.39884451712869</v>
+        <v>-109.5953780685138</v>
       </c>
       <c r="C22">
-        <v>656</v>
+        <v>2624</v>
       </c>
       <c r="D22">
-        <v>-0.04176653127611082</v>
+        <v>-0.04176653127611044</v>
       </c>
       <c r="E22">
-        <v>-27.39884451712869</v>
+        <v>-109.5953780685138</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -891,16 +891,16 @@
         <v>26</v>
       </c>
       <c r="B23">
-        <v>4.769545678384183</v>
+        <v>19.07818271353684</v>
       </c>
       <c r="C23">
-        <v>307</v>
+        <v>1228</v>
       </c>
       <c r="D23">
-        <v>0.01553597940841753</v>
+        <v>0.01553597940841762</v>
       </c>
       <c r="E23">
-        <v>4.769545678384183</v>
+        <v>19.07818271353684</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -908,16 +908,16 @@
         <v>27</v>
       </c>
       <c r="B24">
-        <v>-35.29970888763336</v>
+        <v>-141.1988355505335</v>
       </c>
       <c r="C24">
-        <v>489</v>
+        <v>1956</v>
       </c>
       <c r="D24">
-        <v>-0.07218754373749155</v>
+        <v>-0.07218754373749157</v>
       </c>
       <c r="E24">
-        <v>-35.29970888763336</v>
+        <v>-141.1988355505335</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -925,16 +925,16 @@
         <v>28</v>
       </c>
       <c r="B25">
-        <v>5.235910872279911</v>
+        <v>20.9436434891197</v>
       </c>
       <c r="C25">
-        <v>352</v>
+        <v>1408</v>
       </c>
       <c r="D25">
-        <v>0.01487474679624975</v>
+        <v>0.01487474679624979</v>
       </c>
       <c r="E25">
-        <v>5.235910872279911</v>
+        <v>20.9436434891197</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -942,16 +942,16 @@
         <v>29</v>
       </c>
       <c r="B26">
-        <v>-70.63207071307346</v>
+        <v>-282.5282828522926</v>
       </c>
       <c r="C26">
-        <v>735</v>
+        <v>2940</v>
       </c>
       <c r="D26">
-        <v>-0.09609805539193668</v>
+        <v>-0.09609805539193625</v>
       </c>
       <c r="E26">
-        <v>-70.63207071307346</v>
+        <v>-282.5282828522926</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -959,16 +959,16 @@
         <v>30</v>
       </c>
       <c r="B27">
-        <v>-14.81480351482496</v>
+        <v>-59.25921405929971</v>
       </c>
       <c r="C27">
-        <v>311</v>
+        <v>1244</v>
       </c>
       <c r="D27">
-        <v>-0.04763602416342432</v>
+        <v>-0.0476360241634242</v>
       </c>
       <c r="E27">
-        <v>-14.81480351482496</v>
+        <v>-59.25921405929971</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -976,16 +976,16 @@
         <v>31</v>
       </c>
       <c r="B28">
-        <v>-56.72284817988363</v>
+        <v>-226.8913927195349</v>
       </c>
       <c r="C28">
-        <v>407</v>
+        <v>1628</v>
       </c>
       <c r="D28">
-        <v>-0.1393681773461514</v>
+        <v>-0.1393681773461516</v>
       </c>
       <c r="E28">
-        <v>-56.72284817988363</v>
+        <v>-226.8913927195349</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -993,16 +993,16 @@
         <v>32</v>
       </c>
       <c r="B29">
-        <v>-112.1140192001013</v>
+        <v>-448.4560768004027</v>
       </c>
       <c r="C29">
-        <v>624</v>
+        <v>2496</v>
       </c>
       <c r="D29">
-        <v>-0.1796699025642649</v>
+        <v>-0.1796699025642639</v>
       </c>
       <c r="E29">
-        <v>-112.1140192001013</v>
+        <v>-448.4560768004027</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1010,16 +1010,16 @@
         <v>33</v>
       </c>
       <c r="B30">
-        <v>47.89178163639323</v>
+        <v>191.5671265455729</v>
       </c>
       <c r="C30">
-        <v>1645</v>
+        <v>6580</v>
       </c>
       <c r="D30">
         <v>0.02911354506771625</v>
       </c>
       <c r="E30">
-        <v>47.89178163639323</v>
+        <v>191.5671265455729</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1027,16 +1027,16 @@
         <v>34</v>
       </c>
       <c r="B31">
-        <v>-21.48936315323328</v>
+        <v>-85.95745261293301</v>
       </c>
       <c r="C31">
-        <v>196</v>
+        <v>784</v>
       </c>
       <c r="D31">
-        <v>-0.1096396079246596</v>
+        <v>-0.1096396079246594</v>
       </c>
       <c r="E31">
-        <v>-21.48936315323328</v>
+        <v>-85.95745261293301</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1044,16 +1044,16 @@
         <v>35</v>
       </c>
       <c r="B32">
-        <v>-25.66319643063951</v>
+        <v>-102.6527857225576</v>
       </c>
       <c r="C32">
-        <v>767</v>
+        <v>3068</v>
       </c>
       <c r="D32">
-        <v>-0.03345918700213756</v>
+        <v>-0.03345918700213742</v>
       </c>
       <c r="E32">
-        <v>-25.66319643063951</v>
+        <v>-102.6527857225576</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1061,16 +1061,16 @@
         <v>36</v>
       </c>
       <c r="B33">
-        <v>-32.21704538325312</v>
+        <v>-128.8681815330119</v>
       </c>
       <c r="C33">
-        <v>429</v>
+        <v>1716</v>
       </c>
       <c r="D33">
-        <v>-0.07509800788637092</v>
+        <v>-0.0750980078863706</v>
       </c>
       <c r="E33">
-        <v>-32.21704538325312</v>
+        <v>-128.8681815330119</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1078,16 +1078,16 @@
         <v>37</v>
       </c>
       <c r="B34">
-        <v>-90.91604106998062</v>
+        <v>-363.6641642799185</v>
       </c>
       <c r="C34">
-        <v>725</v>
+        <v>2900</v>
       </c>
       <c r="D34">
-        <v>-0.125401435958594</v>
+        <v>-0.1254014359585926</v>
       </c>
       <c r="E34">
-        <v>-90.91604106998062</v>
+        <v>-363.6641642799185</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1095,16 +1095,16 @@
         <v>38</v>
       </c>
       <c r="B35">
-        <v>-31.08809340484496</v>
+        <v>-124.3523736193784</v>
       </c>
       <c r="C35">
-        <v>495</v>
+        <v>1980</v>
       </c>
       <c r="D35">
-        <v>-0.06280422910069688</v>
+        <v>-0.06280422910069618</v>
       </c>
       <c r="E35">
-        <v>-31.08809340484496</v>
+        <v>-124.3523736193784</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1112,16 +1112,16 @@
         <v>39</v>
       </c>
       <c r="B36">
-        <v>14.61025160509103</v>
+        <v>58.44100642036419</v>
       </c>
       <c r="C36">
-        <v>423</v>
+        <v>1692</v>
       </c>
       <c r="D36">
-        <v>0.03453960190328847</v>
+        <v>0.03453960190328853</v>
       </c>
       <c r="E36">
-        <v>14.61025160509103</v>
+        <v>58.44100642036419</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1129,16 +1129,16 @@
         <v>40</v>
       </c>
       <c r="B37">
-        <v>12.00563687872124</v>
+        <v>48.02254751488483</v>
       </c>
       <c r="C37">
-        <v>723</v>
+        <v>2892</v>
       </c>
       <c r="D37">
-        <v>0.01660530688619811</v>
+        <v>0.01660530688619808</v>
       </c>
       <c r="E37">
-        <v>12.00563687872124</v>
+        <v>48.02254751488483</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1146,16 +1146,16 @@
         <v>41</v>
       </c>
       <c r="B38">
-        <v>-22.24308030939039</v>
+        <v>-88.97232123756133</v>
       </c>
       <c r="C38">
-        <v>184</v>
+        <v>736</v>
       </c>
       <c r="D38">
-        <v>-0.1208863060292956</v>
+        <v>-0.1208863060292953</v>
       </c>
       <c r="E38">
-        <v>-22.24308030939039</v>
+        <v>-88.97232123756133</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1163,16 +1163,16 @@
         <v>42</v>
       </c>
       <c r="B39">
-        <v>-126.0295811591185</v>
+        <v>-504.1183246364689</v>
       </c>
       <c r="C39">
-        <v>830</v>
+        <v>3320</v>
       </c>
       <c r="D39">
-        <v>-0.1518428688664079</v>
+        <v>-0.1518428688664063</v>
       </c>
       <c r="E39">
-        <v>-126.0295811591185</v>
+        <v>-504.1183246364689</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1180,16 +1180,16 @@
         <v>43</v>
       </c>
       <c r="B40">
-        <v>-90.53150483595621</v>
+        <v>-362.1260193438251</v>
       </c>
       <c r="C40">
-        <v>856</v>
+        <v>3424</v>
       </c>
       <c r="D40">
         <v>-0.1057611037803227</v>
       </c>
       <c r="E40">
-        <v>-90.53150483595621</v>
+        <v>-362.1260193438251</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1197,16 +1197,16 @@
         <v>44</v>
       </c>
       <c r="B41">
-        <v>-16.39065531181919</v>
+        <v>-65.5626212472756</v>
       </c>
       <c r="C41">
-        <v>535</v>
+        <v>2140</v>
       </c>
       <c r="D41">
-        <v>-0.03063673890059662</v>
+        <v>-0.03063673890059607</v>
       </c>
       <c r="E41">
-        <v>-16.39065531181919</v>
+        <v>-65.5626212472756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>